<commit_message>
feat: format and fixed
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -14,8 +14,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Process/Data ID</t>
+  </si>
+  <si>
+    <t>Case ID</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -35,7 +44,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">select value(AVL_SEQ_NO,0) as AVL_SEQ_NO,int_lim_no,int_lim_year,LOAN_TYPE,digits(LOAN_NO) as LOAN_NO,digits(LOAN_YEAR) as LOAN_YEAR,digits(BRN_CD) as BRN_CD,digits(AC_TYPE) as AC_TYPE,digits(CUST_NO) as CUST_NO,digits(RUN_NO) as RUN_NO,digits(CHK_DIGT) as CHK_DIGT,digits(NOM_AC_TYPE) as NOM_AC_TYPE,digits(NOM_CUST_NO) as NOM_CUST_NO,digits(NOM_RUN_NO) as NOM_RUN_NO,digits(NOM_CHK_DIGT) as NOM_CHK_DIGT,digits(LOAN_AC_TYPE) as LOAN_AC_TYPE,digits(LOAN_CUST_NO) as LOAN_CUST_NO,digits(LOAN_RUN_NO) as LOAN_RUN_NO,digits(LOAN_CHK_DIGT) as LOAN_CHK_DIGT,digits(OVR_AC_TYPE) as OVR_AC_TYPE,digits(OVR_CUST_NO) as OVR_CUST_NO,digits(OVR_RUN_NO) as OVR_RUN_NO,digits(OVR_CHK_DIGT) as OVR_CHK_DIGT,digits(CR_AC_TYPE) as CR_AC_TYPE,digits(CR_CUST_NO) as CR_CUST_NO,digits(CR_RUN_NO) as CR_RUN_NO,digits(CR_CHK_DIGT) as CR_CHK_DIGT,GRANT_DATE,MAT_DATE,LOAN_AMT,FREQ,DOC_TYPE,VALUE(DOC_NO,0) AS DOC_NO,VALUE(DOC_YEAR,0) AS DOC_YEAR,LUM_SUM_INST,VALUE(SECDEP_NO,0) AS SECDEP_NO,VALUE(SECDEP_PERC,0) AS SECDEP_PERC,VALUE(SECDEP_AMT,0) AS SECDEP_AMT,value(SALVAGE_PERC,0) as SALVAGE_PERC,value(Salvage_AMT,0) as Salvage_AMT,digits(Salvage_AC_TYPE) as Salvage_AC_TYPE,digits(Salvage_CUST_NO) as Salvage_CUST_NO,digits(Salvage_RUN_NO) as Salvage_RUN_NO,digits(Salvage_CHK_DIGT) as Salvage_CHK_DIGT, VALUE(TENURE,0) as TENURE,TENURE_UNITS,VALUE(NO_OF_INST,0) as NO_OF_INST,REPAY_FREQ,MORAT_DT,VALUE(MORAT_PRD,0) as MORAT_PRD,INST_SCH_DT,value(status,'') as status,value(accr_amt,0) as accr_amt,value(rec_amt,0) as rec_amt,digits(RT_CODE) as RT_CODE,BASE_RATE,SPREAD_RT,FLOOR_RT,CEILING_RT,MU_RATE,REMARKS ,value(charity_amt,0) as charity_amt from cm_loan_tl where  brn_cd=1024 and full='Y' and (loan_amt=rec_amt) and status='U'  and loan_type in ('LF')  and GRANT_DATE!=date('2024-10-31');
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -91,7 +100,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">actions: </t>
+      <t xml:space="preserve">Actions: </t>
     </r>
     <r>
       <rPr>
@@ -123,9 +132,190 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t xml:space="preserve">1
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Data ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">U.A.28.79.D.3
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Process Step ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">P.A.28.79.D.3
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Case ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">
 </t>
     </r>
+  </si>
+  <si>
+    <t>P.A.28.79.D.3/U.A.28.79.D.3</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Query: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Class: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">TfinUtil
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Line No: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">8476
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Actions: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">getCustomerInfo
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Screen No: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">1
+</t>
+    </r>
     <r>
       <rPr>
         <b/>
@@ -189,17 +379,212 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t xml:space="preserve">C123
+</t>
+    </r>
+  </si>
+  <si>
+    <t>C123</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Query: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">
 </t>
     </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Class: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Line No: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Actions: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">deleteAccount
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Screen No: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Data ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">D789
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Process Step ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Case ID: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">C456
+</t>
+    </r>
+  </si>
+  <si>
+    <t>D789</t>
+  </si>
+  <si>
+    <t>C456</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -227,8 +612,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,15 +912,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>